<commit_message>
update to ms revision submission
</commit_message>
<xml_diff>
--- a/products/manuscript/supplementary_materials/Supplementary Data Table 10.xlsx
+++ b/products/manuscript/supplementary_materials/Supplementary Data Table 10.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Documents/OSUDocs/Projects/Disease_LHS/GCMP_Global_Disease/products/manuscript/supplementary_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ABBAE1-8218-6047-952A-C8F70E9456E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F495261-DD00-534E-BF47-DC64C33770FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="500" windowWidth="27640" windowHeight="15740" activeTab="1" xr2:uid="{635964DC-1275-F24E-A533-4EEDB34ABDB9}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15740" xr2:uid="{635964DC-1275-F24E-A533-4EEDB34ABDB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 10a" sheetId="1" r:id="rId1"/>
     <sheet name="Table 10b" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -202,44 +202,6 @@
   </si>
   <si>
     <t>delta : 1 (95% CI  0.208000121826252  -  NA )</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Phylogenetic generalized least squares (PGLS) correlations between disease susceptibility and host growth rate in a) all corals (zero </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Endozoicomonas</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> counts included). </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Results generated from the PGLS analysis conducted between disease susceptibility and host growth rate across all coral genera that had growth rate data. Four PGLS models (BM, BM_Lambda, BM_Kappa, BM_Delta) were run where parameters were either set to 1 or maximum liklelihood (ML) (see Supplementary Data Table 12 for explanations of parameters). Best model designation is based on the lowest AIC score of the 4 models.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -320,7 +282,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>present and growth rate data. Four PGLS models (BM, BM_Lambda, BM_Kappa, BM_Delta) were run where parameteres were either set to 1 or maximum liklelihood (ML) (see Supplementary Data Table 12 for explanations of parameters). Best model designation is based on the lowest AIC score of the 4 models.</t>
+      <t>present and growth rate data. Four PGLS models (BM, BM_Lambda, BM_Kappa, BM_Delta) were run where parameteres were either set to 1 or maximum liklelihood (ML) (see Supplementary Data Table 13 for explanations of parameters). Best model designation is based on the lowest AIC score of the 4 models.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Phylogenetic generalized least squares (PGLS) correlations between disease susceptibility and host growth rate in a) all corals (zero </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Endozoicomonas</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> counts included). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Results generated from the PGLS analysis conducted between disease susceptibility and host growth rate across all coral genera that had growth rate data. Four PGLS models (BM, BM_Lambda, BM_Kappa, BM_Delta) were run where parameters were either set to 1 or maximum liklelihood (ML) (see Supplementary Data Table 13 for explanations of parameters). Best model designation is based on the lowest AIC score of the 4 models.</t>
     </r>
   </si>
 </sst>
@@ -437,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -477,7 +477,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -583,7 +583,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -725,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -735,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06CC3E0-6C45-264B-AC77-3286BEF35D46}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
@@ -761,7 +761,7 @@
     </row>
     <row r="2" spans="1:24" ht="85.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1170,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED5225F-D3DA-C245-BFD4-0902077852FF}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="2" spans="1:24" ht="85.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>

</xml_diff>